<commit_message>
Recalculo con abono del 19 nov.
</commit_message>
<xml_diff>
--- a/resultado.xlsx
+++ b/resultado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpatr\Documents\nodejs\prestaApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DB7AB7-2C0A-452B-973E-6D8157425E1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF11305-B552-4693-84D7-3507C82B1405}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -94,25 +94,13 @@
     <t>tiempo(dias)</t>
   </si>
   <si>
-    <t>Registro automatizado al 19-dic-2019</t>
-  </si>
-  <si>
-    <t>Abono</t>
-  </si>
-  <si>
-    <t>Monto</t>
-  </si>
-  <si>
-    <t>Fecha ingreso</t>
-  </si>
-  <si>
-    <t>Observacion</t>
-  </si>
-  <si>
-    <t>Por indicar a que contrato se abona</t>
-  </si>
-  <si>
     <t>TERMINADO</t>
+  </si>
+  <si>
+    <t>ApoyoMutuoI-004</t>
+  </si>
+  <si>
+    <t>Registro automatizado al 30-dic-2019</t>
   </si>
 </sst>
 </file>
@@ -120,14 +108,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00_ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -196,34 +191,34 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -501,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P22"/>
+  <dimension ref="B1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -528,8 +523,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" s="8" t="s">
-        <v>24</v>
+      <c r="B1" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:16">
@@ -592,10 +587,10 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>0.12</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -619,11 +614,11 @@
       <c r="N4" s="3">
         <v>2380.9499999999998</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <v>1243.05</v>
       </c>
-      <c r="P4" s="12" t="s">
-        <v>30</v>
+      <c r="P4" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:16">
@@ -639,10 +634,10 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>0.12</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>30</v>
       </c>
       <c r="H5" s="2">
@@ -666,11 +661,11 @@
       <c r="N5" s="3">
         <v>884.95</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9">
         <v>497.32159999999999</v>
       </c>
-      <c r="P5" s="12" t="s">
-        <v>30</v>
+      <c r="P5" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:16">
@@ -686,17 +681,17 @@
       <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="10">
         <v>0.12</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="10">
         <v>30</v>
       </c>
       <c r="H6" s="2">
         <v>43799</v>
       </c>
-      <c r="I6" t="s">
-        <v>14</v>
+      <c r="I6" s="2">
+        <v>43818</v>
       </c>
       <c r="J6">
         <v>19</v>
@@ -711,45 +706,45 @@
         <v>18</v>
       </c>
       <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="5">
+        <v>479.81</v>
+      </c>
+      <c r="O6" s="9">
         <v>535.11631999999997</v>
       </c>
-      <c r="P6" s="9" t="s">
-        <v>20</v>
+      <c r="P6" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D7">
-        <v>3000</v>
+        <v>55.61</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="1">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="G7" s="1">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2">
-        <v>43796</v>
+        <v>43818</v>
       </c>
       <c r="I7" t="s">
         <v>14</v>
       </c>
       <c r="J7">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K7" s="6">
-        <v>412.5</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="L7" t="s">
         <v>17</v>
@@ -761,52 +756,69 @@
         <v>0</v>
       </c>
       <c r="O7" s="5">
-        <v>3412.5</v>
-      </c>
-      <c r="P7" s="9" t="s">
+        <v>58.05</v>
+      </c>
+      <c r="P7" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:16">
-      <c r="H8" s="2"/>
-      <c r="K8" s="6"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="10" spans="2:16">
-      <c r="B10" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16">
-      <c r="B11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="2"/>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>3000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G8" s="1">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2">
+        <v>43796</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>32</v>
+      </c>
+      <c r="K8" s="6">
+        <v>396</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
+        <v>3396</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
+      <c r="H9" s="2"/>
+      <c r="K9" s="6"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="12" spans="2:16">
-      <c r="B12">
-        <v>479.51</v>
-      </c>
-      <c r="C12" s="2">
-        <v>43818</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16">
-      <c r="B13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="2:16">
-      <c r="B14" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6">
-      <c r="F22" s="7"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Actualizacion pendiente al 09-Ene-2020
</commit_message>
<xml_diff>
--- a/resultado.xlsx
+++ b/resultado.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpatr\Documents\nodejs\prestaApp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF11305-B552-4693-84D7-3507C82B1405}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Resultado" sheetId="2" r:id="rId1"/>
@@ -22,6 +16,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
+    <t>Registro automatizado al 09-ene-2020</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
     <t>porcentajeInteres</t>
   </si>
   <si>
+    <t>tiempo(dias)</t>
+  </si>
+  <si>
     <t>fechaInicio</t>
   </si>
   <si>
@@ -79,38 +79,36 @@
     <t>Jorge(Papa)</t>
   </si>
   <si>
+    <t>TERMINADO</t>
+  </si>
+  <si>
     <t>ApoyoMutuoI-002</t>
   </si>
   <si>
+    <t>ApoyoMutuoI-003</t>
+  </si>
+  <si>
+    <t>ApoyoMutuoI-004</t>
+  </si>
+  <si>
     <t>REGISTRADO</t>
   </si>
   <si>
     <t>ApoyoMutuoII-001</t>
-  </si>
-  <si>
-    <t>ApoyoMutuoI-003</t>
-  </si>
-  <si>
-    <t>tiempo(dias)</t>
-  </si>
-  <si>
-    <t>TERMINADO</t>
-  </si>
-  <si>
-    <t>ApoyoMutuoI-004</t>
-  </si>
-  <si>
-    <t>Registro automatizado al 30-dic-2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,26 +120,163 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,18 +291,204 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -175,9 +496,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -185,54 +748,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
+    <cellStyle name="Coma" xfId="6" builtinId="3"/>
+    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
+    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21"/>
+    <cellStyle name="Nota" xfId="11" builtinId="10"/>
+    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
+    <cellStyle name="Título" xfId="14" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
+    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
+    <cellStyle name="Total" xfId="22" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
+    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
+    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
+    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
+    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
+    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
+    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
+    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
+    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -490,113 +1097,113 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.43809523809524" customWidth="1"/>
+    <col min="2" max="2" width="19.552380952381" customWidth="1"/>
+    <col min="3" max="3" width="15.8857142857143" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="15.4380952380952" customWidth="1"/>
+    <col min="7" max="7" width="11.1047619047619" customWidth="1"/>
+    <col min="8" max="8" width="10.8857142857143" customWidth="1"/>
+    <col min="9" max="9" width="9.66666666666667" customWidth="1"/>
+    <col min="10" max="10" width="11.1047619047619" customWidth="1"/>
+    <col min="11" max="11" width="15.8857142857143" customWidth="1"/>
+    <col min="12" max="12" width="12.7809523809524" customWidth="1"/>
+    <col min="13" max="13" width="10.6666666666667" customWidth="1"/>
+    <col min="14" max="14" width="11.6666666666667" customWidth="1"/>
+    <col min="15" max="15" width="17.2190476190476" customWidth="1"/>
+    <col min="16" max="16" width="11.552380952381" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16">
-      <c r="B1" s="12" t="s">
-        <v>26</v>
+    <row r="1" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:16">
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="P3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:16">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>3000</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="10">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2">
         <v>0.12</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="2">
         <v>30</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="3">
         <v>43771</v>
       </c>
       <c r="J4">
@@ -606,44 +1213,44 @@
         <v>624</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="3">
-        <v>2380.9499999999998</v>
-      </c>
-      <c r="O4" s="9">
+        <v>20</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2380.95</v>
+      </c>
+      <c r="O4" s="8">
         <v>1243.05</v>
       </c>
-      <c r="P4" s="11" t="s">
-        <v>24</v>
+      <c r="P4" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:16">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>1243.05</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="10">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2">
         <v>0.12</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="2">
         <v>30</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>43771</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>43799</v>
       </c>
       <c r="J5">
@@ -653,175 +1260,176 @@
         <v>139.2216</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="3">
+        <v>20</v>
+      </c>
+      <c r="N5" s="7">
         <v>884.95</v>
       </c>
-      <c r="O5" s="9">
-        <v>497.32159999999999</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>24</v>
+      <c r="O5" s="8">
+        <v>497.3216</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:16">
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
       </c>
       <c r="D6">
         <v>497.32</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="10">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2">
         <v>0.12</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="2">
         <v>30</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>43799</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <v>43818</v>
       </c>
       <c r="J6">
         <v>19</v>
       </c>
       <c r="K6" s="6">
-        <v>37.796320000000001</v>
+        <v>37.79632</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="3">
+        <v>20</v>
+      </c>
+      <c r="N6" s="7">
         <v>479.81</v>
       </c>
-      <c r="O6" s="9">
-        <v>535.11631999999997</v>
-      </c>
-      <c r="P6" s="11" t="s">
-        <v>24</v>
+      <c r="O6" s="8">
+        <v>535.11632</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>55.61</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4">
         <v>0.12</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>30</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>43818</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J7">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="K7" s="6">
-        <v>2.4500000000000002</v>
+        <v>4.67</v>
       </c>
       <c r="L7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" s="3">
+        <v>20</v>
+      </c>
+      <c r="N7" s="7">
         <v>0</v>
       </c>
-      <c r="O7" s="5">
-        <v>58.05</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>20</v>
+      <c r="O7" s="10">
+        <v>60.28</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:16">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>3000</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1">
+        <v>17</v>
+      </c>
+      <c r="F8" s="4">
         <v>0.12</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="4">
         <v>30</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>43796</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J8">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="K8" s="6">
-        <v>396</v>
+        <v>516</v>
       </c>
       <c r="L8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" s="3">
+        <v>20</v>
+      </c>
+      <c r="N8" s="7">
         <v>0</v>
       </c>
-      <c r="O8" s="5">
-        <v>3396</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>20</v>
+      <c r="O8" s="10">
+        <v>3516</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
-      <c r="H9" s="2"/>
+    <row r="9" spans="8:15">
+      <c r="H9" s="3"/>
       <c r="K9" s="6"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="12"/>
     </row>
-    <row r="12" spans="2:16">
-      <c r="F12" s="12"/>
+    <row r="12" spans="6:6">
+      <c r="F12" s="1"/>
     </row>
     <row r="17" spans="6:6">
-      <c r="F17" s="7"/>
+      <c r="F17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>